<commit_message>
Third Commit (Ruli) - katalon bio farma v.01
</commit_message>
<xml_diff>
--- a/Document/MataUang_DataIntegrasi.xlsx
+++ b/Document/MataUang_DataIntegrasi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Katalon Studio\Bio-Farma\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5CDED-E54F-4BB7-BE02-56B76EE7ED01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1D4509-3CDF-4531-993E-D37AD3F3185A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,34 +178,34 @@
     <t>PT Industri Nuklir Indonesia (Persero)</t>
   </si>
   <si>
-    <t>IDR</t>
-  </si>
-  <si>
     <t>Rupiah</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>US Dollar</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>Euro</t>
   </si>
   <si>
-    <t>EGP</t>
-  </si>
-  <si>
     <t>Pound</t>
   </si>
   <si>
     <t>Won</t>
   </si>
   <si>
-    <t>KPW</t>
+    <t>IDR-AutomatedTest</t>
+  </si>
+  <si>
+    <t>USD-AutomatedTest</t>
+  </si>
+  <si>
+    <t>EUR-AutomatedTest</t>
+  </si>
+  <si>
+    <t>EGP-AutomatedTest</t>
+  </si>
+  <si>
+    <t>KPW-AutomatedTest</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,10 +620,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,10 +634,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,10 +648,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>